<commit_message>
un peu trop de chose modifier pour les décrires donc BD et DCC et DCR et je sais plus et JE
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01_JE.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01_JE.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\GitHub\Projet\Sprint 1\Package 1\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
     <sheet name="tblClassification" sheetId="1" r:id="rId1"/>
     <sheet name="tblGenre" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,9 +52,6 @@
     <t>Everyone 10+</t>
   </si>
   <si>
-    <t>E 10+</t>
-  </si>
-  <si>
     <t>Enfants de 10 ans et plus</t>
   </si>
   <si>
@@ -229,6 +221,9 @@
   </si>
   <si>
     <t>RPG Gestion</t>
+  </si>
+  <si>
+    <t>E10</t>
   </si>
 </sst>
 </file>
@@ -569,7 +564,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -579,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,57 +620,57 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
         <v>61</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -687,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,13 +695,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -714,7 +709,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -722,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -730,7 +725,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -738,7 +733,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -746,7 +741,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -754,7 +749,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -762,7 +757,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -770,7 +765,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -778,7 +773,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -786,7 +781,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -794,7 +789,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -802,7 +797,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -810,7 +805,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -818,7 +813,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -826,7 +821,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -834,7 +829,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -842,7 +837,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -850,7 +845,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -858,7 +853,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -866,7 +861,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -874,7 +869,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -882,7 +877,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -890,7 +885,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -898,7 +893,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -906,7 +901,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -914,7 +909,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -922,7 +917,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -930,7 +925,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -938,7 +933,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -946,7 +941,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -954,7 +949,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -962,7 +957,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -970,7 +965,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -978,7 +973,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -986,7 +981,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -994,7 +989,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -1002,7 +997,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1010,7 +1005,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -1018,7 +1013,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -1026,7 +1021,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -1034,7 +1029,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -1042,7 +1037,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test de correction dla marde que j'ai fait
La marde a seulement rapport avec la fucking bd de merde
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01_JE.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01_JE.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\GitHub\Projet\Sprint 1\Package 1\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="9348" tabRatio="730" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="9348" tabRatio="730" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="tblMode" sheetId="11" r:id="rId1"/>
-    <sheet name="C tblSysExp" sheetId="3" r:id="rId2"/>
-    <sheet name="C tblTheme" sheetId="4" r:id="rId3"/>
-    <sheet name="C tblClassification" sheetId="1" r:id="rId4"/>
-    <sheet name="C tblMode" sheetId="5" r:id="rId5"/>
-    <sheet name="C tblGenre" sheetId="2" r:id="rId6"/>
-    <sheet name="B tblJeu" sheetId="6" r:id="rId7"/>
-    <sheet name="B tblThemeJeu" sheetId="7" r:id="rId8"/>
-    <sheet name="tblVersion" sheetId="10" r:id="rId9"/>
-    <sheet name="tblJeuSemblable" sheetId="12" r:id="rId10"/>
-    <sheet name="tblPlateformeJeu" sheetId="13" r:id="rId11"/>
+    <sheet name="C tblSysExp" sheetId="3" r:id="rId1"/>
+    <sheet name="C tblTheme" sheetId="4" r:id="rId2"/>
+    <sheet name="C tblClassification" sheetId="1" r:id="rId3"/>
+    <sheet name="C tblMode" sheetId="5" r:id="rId4"/>
+    <sheet name="C tblGenre" sheetId="2" r:id="rId5"/>
+    <sheet name="B tblJeu" sheetId="6" r:id="rId6"/>
+    <sheet name="B tblThemeJeu" sheetId="7" r:id="rId7"/>
+    <sheet name="B tblVersion" sheetId="10" r:id="rId8"/>
+    <sheet name="B tblJeuSemblable" sheetId="12" r:id="rId9"/>
+    <sheet name="B tblPlateformeJeu" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -34,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="665">
   <si>
     <t>CoteESRB</t>
   </si>
@@ -2496,7 +2490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2504,600 +2498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="106.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>510</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>512</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>513</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>16</v>
-      </c>
-      <c r="B5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C46"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>514</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>664</v>
-      </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
-        <v>1</v>
-      </c>
-      <c r="B4" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>1</v>
-      </c>
-      <c r="B5" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
-        <v>2</v>
-      </c>
-      <c r="B7" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
-        <v>2</v>
-      </c>
-      <c r="B8" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>2</v>
-      </c>
-      <c r="B9" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
-        <v>2</v>
-      </c>
-      <c r="B10" s="11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
-        <v>2</v>
-      </c>
-      <c r="B11" s="9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
-        <v>2</v>
-      </c>
-      <c r="B12" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" s="9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" s="9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="B15" s="9">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>4</v>
-      </c>
-      <c r="B16" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>5</v>
-      </c>
-      <c r="B17" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>6</v>
-      </c>
-      <c r="B18" s="9">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>7</v>
-      </c>
-      <c r="B19" s="6">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>8</v>
-      </c>
-      <c r="B20" s="12">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>9</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>9</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>9</v>
-      </c>
-      <c r="B23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>10</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>10</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>10</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>10</v>
-      </c>
-      <c r="B28">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>11</v>
-      </c>
-      <c r="B29">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>11</v>
-      </c>
-      <c r="B30">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>11</v>
-      </c>
-      <c r="B31">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>11</v>
-      </c>
-      <c r="B32">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>12</v>
-      </c>
-      <c r="B33">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>12</v>
-      </c>
-      <c r="B34">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>12</v>
-      </c>
-      <c r="B35">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>12</v>
-      </c>
-      <c r="B36">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>13</v>
-      </c>
-      <c r="B37">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>13</v>
-      </c>
-      <c r="B38">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>13</v>
-      </c>
-      <c r="B39">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>13</v>
-      </c>
-      <c r="B40">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>14</v>
-      </c>
-      <c r="B41">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>14</v>
-      </c>
-      <c r="B42">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>15</v>
-      </c>
-      <c r="B43">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>15</v>
-      </c>
-      <c r="B44">
-        <v>16</v>
-      </c>
-      <c r="C44" s="13"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>16</v>
-      </c>
-      <c r="B45">
-        <v>15</v>
-      </c>
-      <c r="C45" s="13"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>16</v>
-      </c>
-      <c r="B46">
-        <v>16</v>
-      </c>
-      <c r="C46" s="13"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F83"/>
   <sheetViews>
     <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4530,7 +3934,398 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>2</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>2</v>
+      </c>
+      <c r="B9" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>2</v>
+      </c>
+      <c r="B11" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>2</v>
+      </c>
+      <c r="B12" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" s="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20" s="12">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>11</v>
+      </c>
+      <c r="B29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>11</v>
+      </c>
+      <c r="B31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>11</v>
+      </c>
+      <c r="B32">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>12</v>
+      </c>
+      <c r="B33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>12</v>
+      </c>
+      <c r="B35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>12</v>
+      </c>
+      <c r="B36">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>13</v>
+      </c>
+      <c r="B37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>13</v>
+      </c>
+      <c r="B38">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>13</v>
+      </c>
+      <c r="B39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>14</v>
+      </c>
+      <c r="B41">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>14</v>
+      </c>
+      <c r="B42">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>15</v>
+      </c>
+      <c r="B43">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>15</v>
+      </c>
+      <c r="B44">
+        <v>16</v>
+      </c>
+      <c r="C44" s="13"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>16</v>
+      </c>
+      <c r="B45">
+        <v>15</v>
+      </c>
+      <c r="C45" s="13"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>16</v>
+      </c>
+      <c r="B46">
+        <v>16</v>
+      </c>
+      <c r="C46" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C337"/>
   <sheetViews>
@@ -7266,7 +7061,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -7374,7 +7169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -7449,7 +7244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
@@ -7826,11 +7621,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -8240,7 +8035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
@@ -8431,7 +8226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
@@ -9288,4 +9083,128 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fuck Srry pour sa
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01_JE.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01_JE.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\Projet\Sprint 1\Package 1\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="9348" tabRatio="730" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="9348" tabRatio="730" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="C tblSysExp" sheetId="3" r:id="rId1"/>
@@ -17,6 +22,9 @@
     <sheet name="B tblVersion" sheetId="10" r:id="rId8"/>
     <sheet name="B tblJeuSemblable" sheetId="12" r:id="rId9"/>
     <sheet name="B tblPlateformeJeu" sheetId="13" r:id="rId10"/>
+    <sheet name="C tblPlateformeSysExp" sheetId="14" r:id="rId11"/>
+    <sheet name="C tblPlateforme" sheetId="15" r:id="rId12"/>
+    <sheet name="C tblCategorie" sheetId="16" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -28,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="813">
   <si>
     <t>CoteESRB</t>
   </si>
@@ -2023,13 +2031,457 @@
   </si>
   <si>
     <t>IdPlateforme</t>
+  </si>
+  <si>
+    <t>IdSysExp</t>
+  </si>
+  <si>
+    <t>PS4, Xbox One, Wii U</t>
+  </si>
+  <si>
+    <t>Console de salon</t>
+  </si>
+  <si>
+    <t>ConSal</t>
+  </si>
+  <si>
+    <t>PS Vita, 3DS</t>
+  </si>
+  <si>
+    <t>Console Portative</t>
+  </si>
+  <si>
+    <t>ConPort</t>
+  </si>
+  <si>
+    <t>Tablette Windows,Ipad, Ipad2,Nexus 4, Nexus 5,Galaxy Tab 4, Galaxy Tab 3, Galaxy Tab S, Galaxy Tab A, etc.</t>
+  </si>
+  <si>
+    <t>Tablette intelligente</t>
+  </si>
+  <si>
+    <t>Tablet</t>
+  </si>
+  <si>
+    <t>Ordinateur de Bureau</t>
+  </si>
+  <si>
+    <t>PCBur</t>
+  </si>
+  <si>
+    <t>Ordinateur Portable</t>
+  </si>
+  <si>
+    <t>PCPort</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S6, Galaxy Note 5,Iphone 5, Iphone 6</t>
+  </si>
+  <si>
+    <t>Téléphone intelligent</t>
+  </si>
+  <si>
+    <t>CommentaireCategorie</t>
+  </si>
+  <si>
+    <t>DescCategorie</t>
+  </si>
+  <si>
+    <t>CodeCategorie</t>
+  </si>
+  <si>
+    <t>Alien</t>
+  </si>
+  <si>
+    <t>Alienware15</t>
+  </si>
+  <si>
+    <t>4e génération Intel Core jusqu'à i7</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>DDR4 de 8 Go 2133MHz (4Gox2)</t>
+  </si>
+  <si>
+    <t>Disque dur SATA de 1 To à 7 200 tr/min et 6 Gbit/s</t>
+  </si>
+  <si>
+    <t>Portable Élite</t>
+  </si>
+  <si>
+    <t>NVIDIA® GeForce® GTX 965M with 2GB GDDR5</t>
+  </si>
+  <si>
+    <t>OptiPlex</t>
+  </si>
+  <si>
+    <t>OptiPlex 3030 tout-en-un</t>
+  </si>
+  <si>
+    <t>Intel® Celeron® G1840</t>
+  </si>
+  <si>
+    <t>Intel Core</t>
+  </si>
+  <si>
+    <t>DDR3L 4 Go3 à 1600 MHz</t>
+  </si>
+  <si>
+    <t>Disque dur de 500Go, 7200 t/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ordinateur d'entreprise  </t>
+  </si>
+  <si>
+    <t>Carte graphique Intel® intégrée</t>
+  </si>
+  <si>
+    <t>Aspire</t>
+  </si>
+  <si>
+    <t>Ordinateur Aspire TC d'Acer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core i5 4e génération d'Intel </t>
+  </si>
+  <si>
+    <t>Aspire TC, Acer</t>
+  </si>
+  <si>
+    <t>8 Go de mémoire vive</t>
+  </si>
+  <si>
+    <t>Disque dur de 1 To</t>
+  </si>
+  <si>
+    <t>Ordinateur moins performante</t>
+  </si>
+  <si>
+    <t>carte graph. HD 4600 Intel</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S5</t>
+  </si>
+  <si>
+    <t>2,5 GHz Quadricoeur</t>
+  </si>
+  <si>
+    <t>Qualcomm MSM8974AC Snapdragon 801</t>
+  </si>
+  <si>
+    <t>16 Go</t>
+  </si>
+  <si>
+    <t>2 Go</t>
+  </si>
+  <si>
+    <t>Téléphone intelligent Android de petit format</t>
+  </si>
+  <si>
+    <t>Micro-SIM (3FF)</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S6</t>
+  </si>
+  <si>
+    <t>octocœur 2.1GHz de 64 bits</t>
+  </si>
+  <si>
+    <t>Exynos 7420</t>
+  </si>
+  <si>
+    <t>32 Go</t>
+  </si>
+  <si>
+    <t>3 Go</t>
+  </si>
+  <si>
+    <t>Téléphone intelligent Android de plus gros format</t>
+  </si>
+  <si>
+    <t>Nano SIM</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>IPhone 5s</t>
+  </si>
+  <si>
+    <t>Double coeur 1.3 GHz Cyclone</t>
+  </si>
+  <si>
+    <t>Puce A7 à architecture 64 bits Coprocesseur de mouvement M7</t>
+  </si>
+  <si>
+    <t>1 Go DDR3</t>
+  </si>
+  <si>
+    <t>16-32 Go</t>
+  </si>
+  <si>
+    <t>Téléphone intelligent Apple d'une version antérieur</t>
+  </si>
+  <si>
+    <t>Nano-SIM</t>
+  </si>
+  <si>
+    <t>IPhone 6</t>
+  </si>
+  <si>
+    <t>Double coeur 1.4 GHz Cyclone</t>
+  </si>
+  <si>
+    <t>Puce A8 à architecture 64 bits Coprocesseur de mouvement M8</t>
+  </si>
+  <si>
+    <t>16-64 Go</t>
+  </si>
+  <si>
+    <t>Téléphone intelligent Apple petit format</t>
+  </si>
+  <si>
+    <t>IPhone 6 Plus</t>
+  </si>
+  <si>
+    <t>Téléphone intelligent Apple de format Moyen</t>
+  </si>
+  <si>
+    <t>Ipad Air</t>
+  </si>
+  <si>
+    <t>Puce A7 à architecture 64 bits</t>
+  </si>
+  <si>
+    <t>Tablette Apple</t>
+  </si>
+  <si>
+    <t>WinSurf</t>
+  </si>
+  <si>
+    <t>Surface Windows</t>
+  </si>
+  <si>
+    <t>NVIDIA TEGRA 3 Quad Core CPU 1.30 GHz</t>
+  </si>
+  <si>
+    <t>Atmel</t>
+  </si>
+  <si>
+    <t>2Go</t>
+  </si>
+  <si>
+    <t>Tablette qui contient Windows 8</t>
+  </si>
+  <si>
+    <t>Galaxy Tab A</t>
+  </si>
+  <si>
+    <t>quadruple coeur APQ 8016 de 1,2 GHz</t>
+  </si>
+  <si>
+    <t>Galaxy Tab motherboard</t>
+  </si>
+  <si>
+    <t>1.5Go</t>
+  </si>
+  <si>
+    <t>128 Go</t>
+  </si>
+  <si>
+    <t>Tablette Android de Grand format</t>
+  </si>
+  <si>
+    <t>Contient une plus grande memoire dû à sa carte mémoire</t>
+  </si>
+  <si>
+    <t>PS4</t>
+  </si>
+  <si>
+    <t>Playstation 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low power x86-64 AMD “Jaguar”, 8 cores    </t>
+  </si>
+  <si>
+    <t>PS4 motherboard</t>
+  </si>
+  <si>
+    <t>GDDR5 8Go</t>
+  </si>
+  <si>
+    <t>500 Go</t>
+  </si>
+  <si>
+    <t>Console salon de Sony la plus récente</t>
+  </si>
+  <si>
+    <t>PSVita</t>
+  </si>
+  <si>
+    <t>Playstation Vita</t>
+  </si>
+  <si>
+    <t>arm cortex A9 quad core up to 2ghz</t>
+  </si>
+  <si>
+    <t>PS Vita motherboard</t>
+  </si>
+  <si>
+    <t>512 Mo</t>
+  </si>
+  <si>
+    <t>4-32 Go</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Console portative de Sonyqui peut se connecter sur le PlayStation Store </t>
+  </si>
+  <si>
+    <t>XboxOne</t>
+  </si>
+  <si>
+    <t>8 Core AMD custom 1.75 GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AMD "Jaguar" Accelerated Processing Unit</t>
+  </si>
+  <si>
+    <t>8Go DDR3</t>
+  </si>
+  <si>
+    <t>Console salon de Microsoft la plus récente</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>Playstation 3</t>
+  </si>
+  <si>
+    <t>Cell Broadband Engine</t>
+  </si>
+  <si>
+    <t>PS3 motherboard</t>
+  </si>
+  <si>
+    <t>256 Mo</t>
+  </si>
+  <si>
+    <t>120 Go</t>
+  </si>
+  <si>
+    <t>Console salon de Sony</t>
+  </si>
+  <si>
+    <t>Xbox360</t>
+  </si>
+  <si>
+    <t>triple coeur 64-bit</t>
+  </si>
+  <si>
+    <t>Winchester</t>
+  </si>
+  <si>
+    <t>512 Mo de GDDR3</t>
+  </si>
+  <si>
+    <t>250 Go</t>
+  </si>
+  <si>
+    <t>Console salon de Microsoft</t>
+  </si>
+  <si>
+    <t>WiiU</t>
+  </si>
+  <si>
+    <t>multicœur de type IBM Power</t>
+  </si>
+  <si>
+    <t>Wii U Mainboard PCB</t>
+  </si>
+  <si>
+    <t>2 Go de DDR3</t>
+  </si>
+  <si>
+    <t>8-32 Go</t>
+  </si>
+  <si>
+    <t>Console Nintendo la plus récente</t>
+  </si>
+  <si>
+    <t>Mac</t>
+  </si>
+  <si>
+    <t>iMac</t>
+  </si>
+  <si>
+    <t>Intel Core i5 de quatrième génération</t>
+  </si>
+  <si>
+    <t>Intel 20" EMC 2133</t>
+  </si>
+  <si>
+    <t>8 Go</t>
+  </si>
+  <si>
+    <t>3 To</t>
+  </si>
+  <si>
+    <t>Ordinateur Apple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARM11 MPCore-based dual-core </t>
+  </si>
+  <si>
+    <t>3DS motherboard</t>
+  </si>
+  <si>
+    <t>32 Mo</t>
+  </si>
+  <si>
+    <t>128 Mo</t>
+  </si>
+  <si>
+    <t>Console Nintendo qui utilise le 3D</t>
+  </si>
+  <si>
+    <t>C'est la petite version de 3DS</t>
+  </si>
+  <si>
+    <t>InfoSupPlateforme</t>
+  </si>
+  <si>
+    <t>DescPlateforme</t>
+  </si>
+  <si>
+    <t>Stockage</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>CarteMere</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>NomPlateforme</t>
+  </si>
+  <si>
+    <t>CodePlateforme</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2045,8 +2497,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4D4D4F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2E3337"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2076,8 +2564,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -2193,12 +2686,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2217,8 +2726,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Commentaire" xfId="2" builtinId="10"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Vérification" xfId="1" builtinId="23"/>
   </cellStyles>
@@ -2490,7 +3012,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3938,8 +4460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4322,6 +4844,978 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>16</v>
+      </c>
+      <c r="B22">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>17</v>
+      </c>
+      <c r="B23">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>18</v>
+      </c>
+      <c r="B24">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" customWidth="1"/>
+    <col min="5" max="5" width="53.77734375" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" customWidth="1"/>
+    <col min="7" max="7" width="41.77734375" customWidth="1"/>
+    <col min="8" max="8" width="60" customWidth="1"/>
+    <col min="9" max="9" width="49" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>684</v>
+      </c>
+      <c r="C2" t="s">
+        <v>685</v>
+      </c>
+      <c r="D2" t="s">
+        <v>686</v>
+      </c>
+      <c r="E2" t="s">
+        <v>687</v>
+      </c>
+      <c r="F2" t="s">
+        <v>688</v>
+      </c>
+      <c r="G2" t="s">
+        <v>689</v>
+      </c>
+      <c r="H2" t="s">
+        <v>690</v>
+      </c>
+      <c r="I2" t="s">
+        <v>691</v>
+      </c>
+      <c r="K2" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>692</v>
+      </c>
+      <c r="C3" t="s">
+        <v>693</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>694</v>
+      </c>
+      <c r="E3" t="s">
+        <v>695</v>
+      </c>
+      <c r="F3" t="s">
+        <v>696</v>
+      </c>
+      <c r="G3" t="s">
+        <v>697</v>
+      </c>
+      <c r="H3" t="s">
+        <v>698</v>
+      </c>
+      <c r="I3" t="s">
+        <v>699</v>
+      </c>
+      <c r="K3" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>700</v>
+      </c>
+      <c r="C4" t="s">
+        <v>701</v>
+      </c>
+      <c r="D4" t="s">
+        <v>702</v>
+      </c>
+      <c r="E4" t="s">
+        <v>703</v>
+      </c>
+      <c r="F4" t="s">
+        <v>704</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>705</v>
+      </c>
+      <c r="H4" t="s">
+        <v>706</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>707</v>
+      </c>
+      <c r="K4" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>708</v>
+      </c>
+      <c r="C5" t="s">
+        <v>709</v>
+      </c>
+      <c r="D5" t="s">
+        <v>710</v>
+      </c>
+      <c r="E5" t="s">
+        <v>711</v>
+      </c>
+      <c r="F5" t="s">
+        <v>712</v>
+      </c>
+      <c r="G5" t="s">
+        <v>713</v>
+      </c>
+      <c r="H5" t="s">
+        <v>714</v>
+      </c>
+      <c r="I5" t="s">
+        <v>715</v>
+      </c>
+      <c r="K5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>708</v>
+      </c>
+      <c r="C6" t="s">
+        <v>716</v>
+      </c>
+      <c r="D6" t="s">
+        <v>717</v>
+      </c>
+      <c r="E6" t="s">
+        <v>718</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>719</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>720</v>
+      </c>
+      <c r="H6" t="s">
+        <v>721</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>722</v>
+      </c>
+      <c r="K6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>723</v>
+      </c>
+      <c r="C7" t="s">
+        <v>724</v>
+      </c>
+      <c r="D7" t="s">
+        <v>725</v>
+      </c>
+      <c r="E7" t="s">
+        <v>726</v>
+      </c>
+      <c r="F7" t="s">
+        <v>727</v>
+      </c>
+      <c r="G7" t="s">
+        <v>728</v>
+      </c>
+      <c r="H7" t="s">
+        <v>729</v>
+      </c>
+      <c r="I7" t="s">
+        <v>730</v>
+      </c>
+      <c r="K7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>723</v>
+      </c>
+      <c r="C8" t="s">
+        <v>731</v>
+      </c>
+      <c r="D8" t="s">
+        <v>732</v>
+      </c>
+      <c r="E8" t="s">
+        <v>733</v>
+      </c>
+      <c r="F8" t="s">
+        <v>727</v>
+      </c>
+      <c r="G8" t="s">
+        <v>734</v>
+      </c>
+      <c r="H8" t="s">
+        <v>735</v>
+      </c>
+      <c r="I8" t="s">
+        <v>730</v>
+      </c>
+      <c r="K8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>723</v>
+      </c>
+      <c r="C9" t="s">
+        <v>736</v>
+      </c>
+      <c r="D9" t="s">
+        <v>732</v>
+      </c>
+      <c r="E9" t="s">
+        <v>733</v>
+      </c>
+      <c r="F9" t="s">
+        <v>727</v>
+      </c>
+      <c r="G9" t="s">
+        <v>734</v>
+      </c>
+      <c r="H9" t="s">
+        <v>737</v>
+      </c>
+      <c r="I9" t="s">
+        <v>730</v>
+      </c>
+      <c r="K9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>723</v>
+      </c>
+      <c r="C10" t="s">
+        <v>738</v>
+      </c>
+      <c r="D10" t="s">
+        <v>725</v>
+      </c>
+      <c r="E10" t="s">
+        <v>739</v>
+      </c>
+      <c r="F10" t="s">
+        <v>727</v>
+      </c>
+      <c r="G10" t="s">
+        <v>728</v>
+      </c>
+      <c r="H10" t="s">
+        <v>740</v>
+      </c>
+      <c r="I10" t="s">
+        <v>687</v>
+      </c>
+      <c r="K10" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>741</v>
+      </c>
+      <c r="C11" t="s">
+        <v>742</v>
+      </c>
+      <c r="D11" t="s">
+        <v>743</v>
+      </c>
+      <c r="E11" t="s">
+        <v>744</v>
+      </c>
+      <c r="F11" t="s">
+        <v>745</v>
+      </c>
+      <c r="G11" t="s">
+        <v>719</v>
+      </c>
+      <c r="H11" t="s">
+        <v>746</v>
+      </c>
+      <c r="I11" t="s">
+        <v>687</v>
+      </c>
+      <c r="K11" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" t="s">
+        <v>747</v>
+      </c>
+      <c r="D12" t="s">
+        <v>748</v>
+      </c>
+      <c r="E12" t="s">
+        <v>749</v>
+      </c>
+      <c r="F12" t="s">
+        <v>750</v>
+      </c>
+      <c r="G12" t="s">
+        <v>751</v>
+      </c>
+      <c r="H12" t="s">
+        <v>752</v>
+      </c>
+      <c r="I12" t="s">
+        <v>753</v>
+      </c>
+      <c r="K12" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>754</v>
+      </c>
+      <c r="C13" t="s">
+        <v>755</v>
+      </c>
+      <c r="D13" t="s">
+        <v>756</v>
+      </c>
+      <c r="E13" t="s">
+        <v>757</v>
+      </c>
+      <c r="F13" t="s">
+        <v>758</v>
+      </c>
+      <c r="G13" t="s">
+        <v>759</v>
+      </c>
+      <c r="H13" t="s">
+        <v>760</v>
+      </c>
+      <c r="I13" t="s">
+        <v>687</v>
+      </c>
+      <c r="K13" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>761</v>
+      </c>
+      <c r="C14" t="s">
+        <v>762</v>
+      </c>
+      <c r="D14" t="s">
+        <v>763</v>
+      </c>
+      <c r="E14" t="s">
+        <v>764</v>
+      </c>
+      <c r="F14" t="s">
+        <v>765</v>
+      </c>
+      <c r="G14" t="s">
+        <v>766</v>
+      </c>
+      <c r="H14" t="s">
+        <v>767</v>
+      </c>
+      <c r="I14" t="s">
+        <v>687</v>
+      </c>
+      <c r="K14" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>768</v>
+      </c>
+      <c r="C15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" t="s">
+        <v>769</v>
+      </c>
+      <c r="E15" t="s">
+        <v>770</v>
+      </c>
+      <c r="F15" t="s">
+        <v>771</v>
+      </c>
+      <c r="G15" t="s">
+        <v>759</v>
+      </c>
+      <c r="H15" t="s">
+        <v>772</v>
+      </c>
+      <c r="I15" t="s">
+        <v>687</v>
+      </c>
+      <c r="K15" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>773</v>
+      </c>
+      <c r="C16" t="s">
+        <v>774</v>
+      </c>
+      <c r="D16" t="s">
+        <v>775</v>
+      </c>
+      <c r="E16" t="s">
+        <v>776</v>
+      </c>
+      <c r="F16" t="s">
+        <v>777</v>
+      </c>
+      <c r="G16" t="s">
+        <v>778</v>
+      </c>
+      <c r="H16" t="s">
+        <v>779</v>
+      </c>
+      <c r="I16" t="s">
+        <v>687</v>
+      </c>
+      <c r="K16" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>780</v>
+      </c>
+      <c r="C17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" t="s">
+        <v>781</v>
+      </c>
+      <c r="E17" t="s">
+        <v>782</v>
+      </c>
+      <c r="F17" t="s">
+        <v>783</v>
+      </c>
+      <c r="G17" t="s">
+        <v>784</v>
+      </c>
+      <c r="H17" t="s">
+        <v>785</v>
+      </c>
+      <c r="I17" t="s">
+        <v>687</v>
+      </c>
+      <c r="K17" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>786</v>
+      </c>
+      <c r="C18" t="s">
+        <v>786</v>
+      </c>
+      <c r="D18" t="s">
+        <v>787</v>
+      </c>
+      <c r="E18" t="s">
+        <v>788</v>
+      </c>
+      <c r="F18" t="s">
+        <v>789</v>
+      </c>
+      <c r="G18" t="s">
+        <v>790</v>
+      </c>
+      <c r="H18" t="s">
+        <v>791</v>
+      </c>
+      <c r="K18" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>792</v>
+      </c>
+      <c r="C19" t="s">
+        <v>793</v>
+      </c>
+      <c r="D19" t="s">
+        <v>794</v>
+      </c>
+      <c r="E19" t="s">
+        <v>795</v>
+      </c>
+      <c r="F19" t="s">
+        <v>796</v>
+      </c>
+      <c r="G19" t="s">
+        <v>797</v>
+      </c>
+      <c r="H19" t="s">
+        <v>798</v>
+      </c>
+      <c r="I19" t="s">
+        <v>687</v>
+      </c>
+      <c r="K19" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" t="s">
+        <v>799</v>
+      </c>
+      <c r="E20" t="s">
+        <v>800</v>
+      </c>
+      <c r="F20" t="s">
+        <v>801</v>
+      </c>
+      <c r="G20" t="s">
+        <v>802</v>
+      </c>
+      <c r="H20" t="s">
+        <v>803</v>
+      </c>
+      <c r="I20" t="s">
+        <v>804</v>
+      </c>
+      <c r="K20" t="s">
+        <v>671</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="87.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>683</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>682</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>680</v>
+      </c>
+      <c r="C2" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>678</v>
+      </c>
+      <c r="B3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>676</v>
+      </c>
+      <c r="B4" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>674</v>
+      </c>
+      <c r="B5" t="s">
+        <v>673</v>
+      </c>
+      <c r="C5" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>671</v>
+      </c>
+      <c r="B6" t="s">
+        <v>670</v>
+      </c>
+      <c r="C6" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>668</v>
+      </c>
+      <c r="B7" t="s">
+        <v>667</v>
+      </c>
+      <c r="C7" t="s">
+        <v>666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
maj DCC et DCR
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01_JE.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01_JE.xlsx
@@ -1,30 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\Projet\Sprint 1\Package 1\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="9348" tabRatio="730" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="9348" tabRatio="930" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="C tblSysExp" sheetId="3" r:id="rId1"/>
-    <sheet name="C tblTheme" sheetId="4" r:id="rId2"/>
-    <sheet name="C tblClassification" sheetId="1" r:id="rId3"/>
-    <sheet name="C tblMode" sheetId="5" r:id="rId4"/>
-    <sheet name="C tblGenre" sheetId="2" r:id="rId5"/>
-    <sheet name="B tblJeu" sheetId="6" r:id="rId6"/>
-    <sheet name="B tblThemeJeu" sheetId="7" r:id="rId7"/>
-    <sheet name="B tblVersion" sheetId="10" r:id="rId8"/>
-    <sheet name="B tblJeuSemblable" sheetId="12" r:id="rId9"/>
-    <sheet name="B tblPlateformeJeu" sheetId="13" r:id="rId10"/>
-    <sheet name="C tblPlateformeSysExp" sheetId="14" r:id="rId11"/>
-    <sheet name="C tblPlateforme" sheetId="15" r:id="rId12"/>
-    <sheet name="C tblCategorie" sheetId="16" r:id="rId13"/>
+    <sheet name="C tblCategorie" sheetId="16" r:id="rId2"/>
+    <sheet name="C tblTheme" sheetId="4" r:id="rId3"/>
+    <sheet name="C tblClassification" sheetId="1" r:id="rId4"/>
+    <sheet name="C tblMode" sheetId="5" r:id="rId5"/>
+    <sheet name="C tblGenre" sheetId="2" r:id="rId6"/>
+    <sheet name="B tblJeu" sheetId="6" r:id="rId7"/>
+    <sheet name="B tblThemeJeu" sheetId="7" r:id="rId8"/>
+    <sheet name="B tblVersion" sheetId="10" r:id="rId9"/>
+    <sheet name="B tblJeuSemblable" sheetId="12" r:id="rId10"/>
+    <sheet name="B tblPlateformeJeu" sheetId="13" r:id="rId11"/>
+    <sheet name="C tblPlateformeSysExp" sheetId="14" r:id="rId12"/>
+    <sheet name="C tblPlateforme" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -36,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="814">
   <si>
     <t>CoteESRB</t>
   </si>
@@ -2475,6 +2470,9 @@
   </si>
   <si>
     <t>CodePlateforme</t>
+  </si>
+  <si>
+    <t>Lieu Caraïbes Plage</t>
   </si>
 </sst>
 </file>
@@ -3012,7 +3010,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4458,6 +4456,130 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4847,7 +4969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -5063,12 +5185,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5729,12 +5851,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5819,12 +5941,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C337"/>
   <sheetViews>
-    <sheetView topLeftCell="A296" workbookViewId="0">
-      <selection activeCell="D326" sqref="D326"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="C203" sqref="C203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7472,7 +7594,7 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>368</v>
+        <v>813</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
@@ -8555,7 +8677,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -8663,7 +8785,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -8738,7 +8860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
@@ -9115,7 +9237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
@@ -9529,12 +9651,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A22"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9720,7 +9842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
@@ -10577,128 +10699,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>16</v>
-      </c>
-      <c r="B5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>